<commit_message>
cognitive service interpretation scoring/benchmark review preprocessing advanced model review blog done deployment azure done
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_7\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5DA89C-FD69-4A54-9CC1-A3C92D13DB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A9828C-3B97-4507-AB90-DAF6670649EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,13 +144,13 @@
     <t>Ajouter un modèle RNN</t>
   </si>
   <si>
-    <t>Accuracy + Matrice de confusion Revoir pour ajouter AUROC ?</t>
-  </si>
-  <si>
-    <t>Faire le script déploiement ML Azure avec MLFLow</t>
-  </si>
-  <si>
-    <t>Rajouter la matrice de confusion et AUROC explicaiton ?</t>
+    <t xml:space="preserve">AUROC + Matrice de confusion </t>
+  </si>
+  <si>
+    <t>Matrice de confusion et AUROC</t>
+  </si>
+  <si>
+    <t>Fait</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,11 +846,11 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C8,C10:C15,C17:C18,C20:C21)</f>
-        <v>0.9642857142857143</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
         <f>AVERAGE(C23:C24)</f>
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -885,7 +885,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>35</v>
@@ -898,12 +898,12 @@
       <c r="C9" s="23"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="2:8" ht="66" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="49.5" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="12">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>36</v>
@@ -959,10 +959,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -1038,10 +1038,10 @@
         <v>23</v>
       </c>
       <c r="C23" s="16">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1049,7 +1049,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="4"/>
     </row>

</xml_diff>